<commit_message>
homestreach of gli program
</commit_message>
<xml_diff>
--- a/GLI_program/plot_working_folder/Tables_Excel_Scratch_Book.xlsx
+++ b/GLI_program/plot_working_folder/Tables_Excel_Scratch_Book.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\GLI_program\plot_working_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CA8C36-4D3E-427A-B54B-F02A4D12F571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129B8703-2B86-4CDA-93F1-B8043CA7650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="345" windowWidth="18900" windowHeight="11505" activeTab="2" xr2:uid="{F9862DA5-5AF3-4862-813A-07A8CFA6BCE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F9862DA5-5AF3-4862-813A-07A8CFA6BCE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Coach_Roster_style" sheetId="3" r:id="rId2"/>
     <sheet name="Attendance" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>School Name</t>
   </si>
@@ -360,12 +361,24 @@
   <si>
     <t>32nd Year (492-592-113)</t>
   </si>
+  <si>
+    <t>Michigan State:</t>
+  </si>
+  <si>
+    <t>Ferris State:</t>
+  </si>
+  <si>
+    <t>Michigan Tech:</t>
+  </si>
+  <si>
+    <t>Alaska:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,8 +509,15 @@
       <color rgb="FFFCC917"/>
       <name val="Exo 2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +569,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBA0C2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4D4D4D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF23A5D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF369A85"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3C8DD0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,7 +742,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,27 +871,27 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -863,6 +907,21 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -872,6 +931,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3C8DD0"/>
+      <color rgb="FF369A85"/>
+      <color rgb="FFF23A5D"/>
+      <color rgb="FF4D4D4D"/>
       <color rgb="FFFCC917"/>
       <color rgb="FFBA0C2F"/>
       <color rgb="FFFFCD00"/>
@@ -1997,29 +2060,29 @@
       <c r="D23" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="49" t="s">
+      <c r="E23" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="50"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.5">
       <c r="C24" s="9"/>
       <c r="D24" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="52"/>
+      <c r="F24" s="51"/>
     </row>
     <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D25" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="54"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.5">
       <c r="D29" s="36" t="s">
@@ -2125,30 +2188,30 @@
       <c r="D40" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="50"/>
+      <c r="F40" s="49"/>
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.5">
       <c r="D41" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="F41" s="52"/>
+      <c r="F41" s="51"/>
       <c r="J41" s="9"/>
     </row>
     <row r="42" spans="4:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D42" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="53" t="s">
+      <c r="E42" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="54"/>
+      <c r="F42" s="53"/>
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.5">
@@ -2161,8 +2224,8 @@
       <c r="J45" s="9"/>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.5">
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.5">
       <c r="D47" s="40" t="s">
@@ -2268,30 +2331,30 @@
       <c r="D58" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="49" t="s">
+      <c r="E58" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F58" s="50"/>
+      <c r="F58" s="49"/>
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.5">
       <c r="D59" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="51" t="s">
+      <c r="E59" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="52"/>
+      <c r="F59" s="51"/>
       <c r="J59" s="9"/>
     </row>
     <row r="60" spans="4:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D60" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E60" s="53" t="s">
+      <c r="E60" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="54"/>
+      <c r="F60" s="53"/>
       <c r="J60" s="9"/>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.5">
@@ -2399,8 +2462,8 @@
       </c>
       <c r="F72" s="27"/>
       <c r="H72" s="7"/>
-      <c r="J72" s="48"/>
-      <c r="K72" s="48"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
     </row>
     <row r="73" spans="4:11" x14ac:dyDescent="0.5">
       <c r="D73" s="45" t="s">
@@ -2433,10 +2496,10 @@
       <c r="D76" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="49" t="s">
+      <c r="E76" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F76" s="50"/>
+      <c r="F76" s="49"/>
       <c r="H76" s="7">
         <v>1975</v>
       </c>
@@ -2450,10 +2513,10 @@
       <c r="D77" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="E77" s="51" t="s">
+      <c r="E77" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F77" s="52"/>
+      <c r="F77" s="51"/>
       <c r="H77" s="7"/>
       <c r="I77" t="s">
         <v>7</v>
@@ -2469,10 +2532,10 @@
       <c r="D78" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E78" s="53" t="s">
+      <c r="E78" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="54"/>
+      <c r="F78" s="53"/>
       <c r="H78" s="7">
         <v>1</v>
       </c>
@@ -2586,21 +2649,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="H89:I89"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="7" scale="29" orientation="portrait" r:id="rId1"/>
@@ -2615,8 +2678,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,4 +2761,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873DEAF-4CB7-48EA-B779-20FF16A0809F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A5:R5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="1.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:18" s="66" customFormat="1" ht="24" x14ac:dyDescent="0.5">
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="63"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="65"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>